<commit_message>
email upload fixed with headers
</commit_message>
<xml_diff>
--- a/D:\test excel\tester2.xlsx
+++ b/D:\test excel\tester2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF26BE4D-FD50-5B46-9454-3F121FFCE9D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376938CB-39EF-2C40-A140-034530C25168}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5020" yWindow="500" windowWidth="25040" windowHeight="13660" xr2:uid="{55A41796-9E0E-C946-9C36-D8E1E97CB43F}"/>
   </bookViews>
@@ -42,13 +42,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Refcode</t>
-  </si>
-  <si>
     <t>2021-05-24 17:39:41</t>
   </si>
   <si>
     <t>Fourth</t>
+  </si>
+  <si>
+    <t>Emails Refcode</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -422,18 +422,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recurring counts added for email in repo and service
</commit_message>
<xml_diff>
--- a/D:\test excel\tester2.xlsx
+++ b/D:\test excel\tester2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376938CB-39EF-2C40-A140-034530C25168}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A248CF-3BF3-7E45-B608-23BF995932CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5020" yWindow="500" windowWidth="25040" windowHeight="13660" xr2:uid="{55A41796-9E0E-C946-9C36-D8E1E97CB43F}"/>
   </bookViews>
@@ -34,28 +34,97 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2021-05-24 17:39:41</t>
-  </si>
-  <si>
-    <t>Fourth</t>
-  </si>
-  <si>
-    <t>Emails Refcode</t>
+    <t>Receipt ID</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Recurring Total Months</t>
+  </si>
+  <si>
+    <t>Recurrence Number</t>
+  </si>
+  <si>
+    <t>Donor First Name</t>
+  </si>
+  <si>
+    <t>Donor Last Name</t>
+  </si>
+  <si>
+    <t>Donor Addr1</t>
+  </si>
+  <si>
+    <t>Donor City</t>
+  </si>
+  <si>
+    <t>Donor State</t>
+  </si>
+  <si>
+    <t>Donor ZIP</t>
+  </si>
+  <si>
+    <t>Donor Country</t>
+  </si>
+  <si>
+    <t>Donor Email</t>
+  </si>
+  <si>
+    <t>Donor Phone</t>
+  </si>
+  <si>
+    <t>Reference Code</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>TestEmail</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>3401 Kessler Boulevard East Dr.</t>
+  </si>
+  <si>
+    <t>Fishers</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>thewzm@gmail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>AB191799309</t>
+  </si>
+  <si>
+    <t>2021-04-25 09:25:55</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -63,13 +132,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,10 +186,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF34990-9F7B-1C4A-9F81-E3F8979EE04C}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -414,29 +531,104 @@
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4">
+        <v>25</v>
+      </c>
+      <c r="D2" s="4">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="4">
+        <v>46220</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="4">
+        <v>3173138391</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{82BD6CC1-F96D-684D-A3D7-C66B25D7F2B7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aggregate functions added to email data
</commit_message>
<xml_diff>
--- a/D:\test excel\tester2.xlsx
+++ b/D:\test excel\tester2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A248CF-3BF3-7E45-B608-23BF995932CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2116382-8368-7B4E-952D-F3361C947541}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5020" yWindow="500" windowWidth="25040" windowHeight="13660" xr2:uid="{55A41796-9E0E-C946-9C36-D8E1E97CB43F}"/>
   </bookViews>
@@ -117,7 +117,7 @@
     <t>AB191799309</t>
   </si>
   <si>
-    <t>2021-04-25 09:25:55</t>
+    <t>2021-06-25 09:25:55</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>

</xml_diff>